<commit_message>
grep and reference edits
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\Rmimix\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkevi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077C6863-1337-4D57-A9F9-0CB7809AABFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E0B6E96-2DC2-4C22-B5B8-2BAEE5A166C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10920" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="1350" yWindow="330" windowWidth="18645" windowHeight="9735" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -99,6 +90,12 @@
   </si>
   <si>
     <t>Mimix version</t>
+  </si>
+  <si>
+    <t>specify exact match by  [grep(paste0("^",scovar[[i]],"$") Runmimix.R  line 114</t>
+  </si>
+  <si>
+    <t>delete head in reference&lt;-(as.numeric(unique(head(tmptreat)[ref_pos])))  Runmimix.R</t>
   </si>
 </sst>
 </file>
@@ -160,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -187,6 +184,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +589,9 @@
       <c r="H3" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="I3" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -614,6 +617,9 @@
       </c>
       <c r="H4" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tests updated in program and results in spreadsheet
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkevi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\Rmimix\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E0B6E96-2DC2-4C22-B5B8-2BAEE5A166C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253865ED-8ADC-445E-BC11-27A6BE2F15A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="330" windowWidth="18645" windowHeight="9735" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="315" yWindow="3960" windowWidth="24990" windowHeight="14115" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -55,9 +58,6 @@
 attempt to select more than one element in vectorIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
     <t>Error in preprodata(data, covar, depvar, treatvar, idvar, timevar, M,  : 
 reference %in% t(ntreat) is not TRUE</t>
   </si>
@@ -96,13 +96,55 @@
   </si>
   <si>
     <t>delete head in reference&lt;-(as.numeric(unique(head(tmptreat)[ref_pos])))  Runmimix.R</t>
+  </si>
+  <si>
+    <t>package RefBasedMI v0.0.18, revised 26/5/2021</t>
+  </si>
+  <si>
+    <t>"Summary of missing data pattern by treat" has treat = 3…2…1 where it should be 1…2…3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study the detailed output from first call to RefBasedMI. </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>"Imputing interim missing values under MAR" omits treat=1 pattern=13 n=1</t>
+  </si>
+  <si>
+    <t>- but has treat the correct way round!</t>
+  </si>
+  <si>
+    <t>otherwise correct</t>
+  </si>
+  <si>
+    <t>"Imputing post-discontinuation missing values under J2R" has treat the wrong way round again</t>
+  </si>
+  <si>
+    <t>Current status</t>
+  </si>
+  <si>
+    <t>OK 28/5/21</t>
+  </si>
+  <si>
+    <t>J2R,CR,CIR=MAR in ref arm</t>
+  </si>
+  <si>
+    <t>Replicate run is within MCSEs</t>
+  </si>
+  <si>
+    <t>Read help file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should K0=1 be the default? gives the wrong impression. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +163,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -186,8 +234,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,10 +560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,34 +576,35 @@
     <col min="3" max="3" width="20.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="42.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.85546875" style="8" customWidth="1"/>
     <col min="8" max="8" width="38.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="40.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="6"/>
+    <col min="10" max="10" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="5"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="G1" s="12"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -561,12 +622,15 @@
         <v>6</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -578,24 +642,27 @@
         <v>44341</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>0</v>
@@ -607,27 +674,167 @@
         <v>44341</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="6" t="s">
-        <v>9</v>
+      <c r="C5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:J2" xr:uid="{89A122F3-6F39-4C48-8DF9-4A2FD0305445}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed testing program, showing error in delta method and some minor issues.
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkevi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\Rmimix\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778BDE03-3531-4953-83AC-34B971DD4C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC02A44-CD0C-4B60-BC88-2F0A09ED05AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="0" windowWidth="18810" windowHeight="10155" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="900" yWindow="180" windowWidth="24990" windowHeight="20535" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={CEA38610-5E45-435D-ABF8-A0C392AE311E}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{CEA38610-5E45-435D-ABF8-A0C392AE311E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    help(RefBasedMI) -&gt; to end -&gt; click index -&gt; click DESCRIPTION -&gt; see "packaged" near end</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -142,13 +160,60 @@
   <si>
     <t>replace interim if  statement to capture interims 
  if ( length(setdiff(c(c_mata_miss[1]:deplen),c_mata_miss)) != 0 ) Runmimix.R</t>
+  </si>
+  <si>
+    <t>package RefBasedMI v0.0.18, packaged 28/5/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run file from the top. Wrong warning in first call to RefBasedMI. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warning should not be output for method=MAR and reference=null:
+"nWARNING !! reference value NULL, required for "J2R","CIR","CR","Causal" "
+</t>
+  </si>
+  <si>
+    <t>also n -&gt; \n</t>
+  </si>
+  <si>
+    <t>not solved 15/7/21</t>
+  </si>
+  <si>
+    <t>clarification 15/7/21: I think K0=0 should be default</t>
+  </si>
+  <si>
+    <t>Sort order after imputation should be same as original</t>
+  </si>
+  <si>
+    <t>original was sorted by id and time, imputed by time and id</t>
+  </si>
+  <si>
+    <t>always sort imputed data by id and time regardless of original sort order?</t>
+  </si>
+  <si>
+    <t>Interim missing values should be imputed identically by different methods</t>
+  </si>
+  <si>
+    <t>Post-discontinuation missing values should be imputed differently by differnet methods even after interim missing values</t>
+  </si>
+  <si>
+    <t>Delta option should change imputed values</t>
+  </si>
+  <si>
+    <t>Causal option should respond to tweaked data</t>
+  </si>
+  <si>
+    <t>has no effect!</t>
+  </si>
+  <si>
+    <t>also need to check changes are correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +241,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -265,6 +336,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="White, Ian" id="{BA034BEB-C5F4-4FE6-8A6C-FF65F4F04F94}" userId="S::rmjwiww@ucl.ac.uk::ef641b7c-88a7-42c7-a687-daf906226e55" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -562,15 +639,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2021-07-15T16:54:35.91" personId="{BA034BEB-C5F4-4FE6-8A6C-FF65F4F04F94}" id="{CEA38610-5E45-435D-ABF8-A0C392AE311E}">
+    <text>help(RefBasedMI) -&gt; to end -&gt; click index -&gt; click DESCRIPTION -&gt; see "packaged" near end</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,6 +846,9 @@
       <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="J7" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -790,6 +878,9 @@
       <c r="I8" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="J8" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -816,6 +907,9 @@
       <c r="H9" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="J9" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -836,13 +930,155 @@
       <c r="F10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>35</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>44392</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:J2" xr:uid="{89A122F3-6F39-4C48-8DF9-4A2FD0305445}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
delta, sort and warning edits
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\Rmimix\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkevi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC02A44-CD0C-4B60-BC88-2F0A09ED05AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50446CC1-DF7F-4F30-806D-9E96EEDB99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="180" windowWidth="24990" windowHeight="20535" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="1230" yWindow="210" windowWidth="19500" windowHeight="10080" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,19 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{CEA38610-5E45-435D-ABF8-A0C392AE311E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     help(RefBasedMI) -&gt; to end -&gt; click index -&gt; click DESCRIPTION -&gt; see "packaged" near end</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -46,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -207,13 +216,30 @@
   </si>
   <si>
     <t>also need to check changes are correct</t>
+  </si>
+  <si>
+    <t>edit to Addelta in utility.R  introduced 
+setdiff(vec_tst,covar) to drop covars
+ in onezero vector</t>
+  </si>
+  <si>
+    <t>still need check changes correct</t>
+  </si>
+  <si>
+    <t>added to Runmimix.R impdatamergeord[order(impdatamergeord[,".imp"],
+impdatamergeord[,idvar]),]
+prior to data output</t>
+  </si>
+  <si>
+    <t>edit !is.null(method) &amp; (method != "MAR")  ) 
+also Warning changed to stop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,12 +267,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,10 +672,10 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,8 +982,11 @@
       <c r="H11" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -988,6 +1011,9 @@
       <c r="H12" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="I12" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1053,6 +1079,12 @@
       </c>
       <c r="H15" s="6" t="s">
         <v>51</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Major tidy up of help file and testing sheet
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkevi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50446CC1-DF7F-4F30-806D-9E96EEDB99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACBE293-3D46-4B2C-9169-51E096A585A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="210" windowWidth="19500" windowHeight="10080" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="26175" windowHeight="9885" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,19 +35,10 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{CEA38610-5E45-435D-ABF8-A0C392AE311E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     help(RefBasedMI) -&gt; to end -&gt; click index -&gt; click DESCRIPTION -&gt; see "packaged" near end</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -55,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -185,9 +176,6 @@
     <t>also n -&gt; \n</t>
   </si>
   <si>
-    <t>not solved 15/7/21</t>
-  </si>
-  <si>
     <t>clarification 15/7/21: I think K0=0 should be default</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
   </si>
   <si>
     <t>Interim missing values should be imputed identically by different methods</t>
-  </si>
-  <si>
-    <t>Post-discontinuation missing values should be imputed differently by differnet methods even after interim missing values</t>
   </si>
   <si>
     <t>Delta option should change imputed values</t>
@@ -223,9 +208,6 @@
  in onezero vector</t>
   </si>
   <si>
-    <t>still need check changes correct</t>
-  </si>
-  <si>
     <t>added to Runmimix.R impdatamergeord[order(impdatamergeord[,".imp"],
 impdatamergeord[,idvar]),]
 prior to data output</t>
@@ -233,6 +215,24 @@
   <si>
     <t>edit !is.null(method) &amp; (method != "MAR")  ) 
 also Warning changed to stop</t>
+  </si>
+  <si>
+    <t>not solved 22/10/2021</t>
+  </si>
+  <si>
+    <t>changed to K0=NULL, K1=NULL</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Post-discontinuation missing values should be imputed differently by different methods even after interim missing values</t>
+  </si>
+  <si>
+    <t>fixed by KM before 22/10/2021</t>
+  </si>
+  <si>
+    <t>fixed by IW 22/10/2021</t>
   </si>
 </sst>
 </file>
@@ -669,13 +669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,6 +820,9 @@
       <c r="F5" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="J5" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -840,6 +843,9 @@
       <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="J6" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -866,8 +872,8 @@
       <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>41</v>
+      <c r="J7" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -898,8 +904,8 @@
       <c r="I8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>41</v>
+      <c r="J8" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -927,8 +933,8 @@
       <c r="H9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>41</v>
+      <c r="J9" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -950,11 +956,17 @@
       <c r="F10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -976,14 +988,17 @@
       <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>40</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1000,19 +1015,22 @@
         <v>44392</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="I12" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1029,11 +1047,14 @@
         <v>44392</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="J13" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1049,11 +1070,14 @@
         <v>44392</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="J14" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1069,22 +1093,22 @@
         <v>44392</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>53</v>
+      <c r="J15" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1101,11 +1125,15 @@
         <v>44392</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="D17" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:J2" xr:uid="{89A122F3-6F39-4C48-8DF9-4A2FD0305445}"/>

</xml_diff>

<commit_message>
Add check of no observed data
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACBE293-3D46-4B2C-9169-51E096A585A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB3873-2111-458E-8FBA-08236074B5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="26175" windowHeight="9885" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -895,17 +895,17 @@
       <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>53</v>
+      <c r="J8" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Almost all tests are passed - update
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB3873-2111-458E-8FBA-08236074B5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAB666C-CEC4-4187-81F4-641696A75A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="22932" yWindow="-204" windowWidth="23256" windowHeight="12576" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -217,9 +217,6 @@
 also Warning changed to stop</t>
   </si>
   <si>
-    <t>not solved 22/10/2021</t>
-  </si>
-  <si>
     <t>changed to K0=NULL, K1=NULL</t>
   </si>
   <si>
@@ -233,6 +230,26 @@
   </si>
   <si>
     <t>fixed by IW 22/10/2021</t>
+  </si>
+  <si>
+    <t>fixed by KM 25/10/2021</t>
+  </si>
+  <si>
+    <t>convert treatvar factor to numeric</t>
+  </si>
+  <si>
+    <t>Ian main testing program 234.R</t>
+  </si>
+  <si>
+    <t>package RefBasedMI v0.0.21, packaged 25/10/2021</t>
+  </si>
+  <si>
+    <t>recoding asthma treatments as 11/12/13 should give same results</t>
+  </si>
+  <si>
+    <t>J2R crashes: 
+Error in paramBiglist[[M * (referindex - 1) + m]] :  attempt to select less than one element in get1index 
+--&gt; error is at l1952, SigmaRefer &lt;- paramBiglist[[M*(referindex-1)+m]][2]</t>
   </si>
 </sst>
 </file>
@@ -672,10 +689,10 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +771,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>8</v>
@@ -786,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>9</v>
@@ -821,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -844,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -864,16 +881,19 @@
         <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>53</v>
+      <c r="I7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -893,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>26</v>
@@ -905,7 +925,7 @@
         <v>36</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -925,16 +945,19 @@
         <v>24</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>53</v>
+      <c r="I9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -954,7 +977,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>35</v>
@@ -963,10 +986,10 @@
         <v>41</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -986,7 +1009,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>39</v>
@@ -998,7 +1021,7 @@
         <v>52</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1018,7 +1041,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>43</v>
@@ -1030,7 +1053,7 @@
         <v>51</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1053,7 +1076,7 @@
         <v>25</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1070,13 +1093,13 @@
         <v>44392</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1096,7 +1119,7 @@
         <v>46</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>48</v>
@@ -1108,7 +1131,7 @@
         <v>50</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1131,9 +1154,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="D17" s="7"/>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="7">
+        <v>44503</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:J2" xr:uid="{89A122F3-6F39-4C48-8DF9-4A2FD0305445}"/>

</xml_diff>

<commit_message>
Update test of fitting MI model to imputed data. Add "twelvetimes" test.
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF5A7A1-A0FD-47C5-9D31-D6ABD53D6AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A662057-A05D-4C8D-B64B-FC721B8AD9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="14595" yWindow="300" windowWidth="14535" windowHeight="12735" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -244,30 +244,63 @@
     <t>package RefBasedMI v0.0.21, packaged 25/10/2021</t>
   </si>
   <si>
-    <t>recoding asthma treatments as 11/12/13 should give same results</t>
-  </si>
-  <si>
     <t>J2R crashes: 
 Error in paramBiglist[[M * (referindex - 1) + m]] :  attempt to select less than one element in get1index 
 --&gt; error is at l1952, SigmaRefer &lt;- paramBiglist[[M*(referindex-1)+m]][2]</t>
   </si>
   <si>
-    <t>Test with many time points e.g. 12</t>
-  </si>
-  <si>
     <t>Get better error messages for syntax errors</t>
   </si>
   <si>
-    <t>.id is not unique in output data so as.mids() fails</t>
-  </si>
-  <si>
     <t>Check MI works with imputed data</t>
   </si>
   <si>
     <t>Error testing program.R</t>
   </si>
   <si>
-    <t>not tested</t>
+    <t>Need an error check: treatvar should be 1/2/…</t>
+  </si>
+  <si>
+    <t>.id was not unique in output data so as.mids() failed</t>
+  </si>
+  <si>
+    <t>fixed by KM 16/11/2021</t>
+  </si>
+  <si>
+    <t>package RefBasedMI v0.0.21, packaged 22/11/2021</t>
+  </si>
+  <si>
+    <t>Check MI gives reasonable answers with imputed data</t>
+  </si>
+  <si>
+    <t>treat is modelled as linear and quadratic terms, unlike in raw data</t>
+  </si>
+  <si>
+    <t>recoding asthma treatments as 11/12/13 should give intelligible error</t>
+  </si>
+  <si>
+    <t>twelevetimes_test.R</t>
+  </si>
+  <si>
+    <t>see file header: wrong failure with 20 indivs/group, code failure with 200/group.</t>
+  </si>
+  <si>
+    <t>Check with 12 time points</t>
+  </si>
+  <si>
+    <t>still a problem 22/11/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is because treat is numeric in the raw data but an ordered factor in the imputed data </t>
+  </si>
+  <si>
+    <t>can be fudged by user using as.numeric() but better to do in program</t>
+  </si>
+  <si>
+    <t>need error checks?</t>
+  </si>
+  <si>
+    <t>unclear what is needed</t>
   </si>
 </sst>
 </file>
@@ -335,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -374,6 +407,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -704,13 +743,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18:E20"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,88 +1210,151 @@
       <c r="F16" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="J16" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="15">
         <v>44503</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="I17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="15">
+        <v>44504</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="7">
-        <v>44504</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G18" s="9"/>
+      <c r="I18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>44522</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="7">
-        <v>44504</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>44522</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <v>44504</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="15">
+        <v>44522</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>66</v>
+      <c r="G21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further testing of v0.0.23
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8434F7-E5B7-4519-B649-2FB138A26C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD97092-CAB7-401C-A6D7-0999BD83C684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="4755" windowWidth="27165" windowHeight="15435" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="5205" yWindow="720" windowWidth="27015" windowHeight="18135" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -244,11 +244,6 @@
     <t>package RefBasedMI v0.0.21, packaged 25/10/2021</t>
   </si>
   <si>
-    <t>J2R crashes: 
-Error in paramBiglist[[M * (referindex - 1) + m]] :  attempt to select less than one element in get1index 
---&gt; error is at l1952, SigmaRefer &lt;- paramBiglist[[M*(referindex-1)+m]][2]</t>
-  </si>
-  <si>
     <t>Get better error messages for syntax errors</t>
   </si>
   <si>
@@ -258,9 +253,6 @@
     <t>Error testing program.R</t>
   </si>
   <si>
-    <t>Need an error check: treatvar should be 1/2/…</t>
-  </si>
-  <si>
     <t>.id was not unique in output data so as.mids() failed</t>
   </si>
   <si>
@@ -279,9 +271,6 @@
     <t>recoding asthma treatments as 11/12/13 should give intelligible error</t>
   </si>
   <si>
-    <t>see file header: wrong failure with 20 indivs/group, code failure with 200/group.</t>
-  </si>
-  <si>
     <t>Check with 12 time points</t>
   </si>
   <si>
@@ -294,20 +283,77 @@
     <t>need error checks?</t>
   </si>
   <si>
-    <t>unclear what is needed</t>
-  </si>
-  <si>
     <t>twelvetimes_test.R</t>
   </si>
   <si>
     <t>still a problem 4/1/2022</t>
+  </si>
+  <si>
+    <t>must be sequential but needn't start at 1 - want a nice check</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>see file header: code failure with 200/group.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed by 29/4/2022 - now works </t>
+  </si>
+  <si>
+    <t>see file header: fails but soldiers on with 20 indivs/group</t>
+  </si>
+  <si>
+    <t>now fails at MVN step, but error message not great</t>
+  </si>
+  <si>
+    <t>OK but prefer to improve error message</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Output: Number of post-discontinuation missing values should be 142</t>
+  </si>
+  <si>
+    <t>reported as 147 (new)</t>
+  </si>
+  <si>
+    <t>package RefBasedMI v0.0.23</t>
+  </si>
+  <si>
+    <t>Sort order of output data set should match original</t>
+  </si>
+  <si>
+    <t>sorted by time id cf original by id time</t>
+  </si>
+  <si>
+    <t>interim missing values should be imputed the same by different methods</t>
+  </si>
+  <si>
+    <t>they differ</t>
+  </si>
+  <si>
+    <t>fixed by 29/4/2022</t>
+  </si>
+  <si>
+    <t>even better, it runs now</t>
+  </si>
+  <si>
+    <t>recoding asthma treatments as 11/12/13 should give same output</t>
+  </si>
+  <si>
+    <t>screen output switches between 1/2/3 and 11/12/13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,13 +382,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -368,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -414,6 +472,21 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,13 +816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,33 +1287,34 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="9" t="s">
+    <row r="17" spans="1:10" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="18">
         <v>44503</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>80</v>
+      <c r="E17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1251,23 +1325,26 @@
         <v>61</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="15">
         <v>44504</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="9"/>
+      <c r="H18" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="I18" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1284,16 +1361,16 @@
         <v>44522</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1301,7 +1378,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1</v>
@@ -1310,55 +1387,179 @@
         <v>44522</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="18">
+        <v>44680</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="F21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="9" t="s">
+      <c r="D22" s="18">
+        <v>44680</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="15">
+        <v>44680</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15">
+        <v>44680</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="15">
-        <v>44522</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J21" s="9" t="s">
+      <c r="G24" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="15">
+        <v>44680</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>80</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="15">
+        <v>44680</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:J2" xr:uid="{89A122F3-6F39-4C48-8DF9-4A2FD0305445}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update Mimix testing summary.xlsx
</commit_message>
<xml_diff>
--- a/test/Mimix testing summary.xlsx
+++ b/test/Mimix testing summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\RefbasedMI\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C04AE8-BDD9-4073-B3DE-4BA101846185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6880B1F1-6B76-4B8D-8384-61ACF15A19B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="345" windowWidth="17820" windowHeight="12360" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8E7B28B-D762-4818-8B67-FEFC4C484397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="103">
   <si>
     <t>package RefBasedMI v0.0.18</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>object output OK, but first output to screen "Summary of missing data pattern by treat:" uses 1/2/3 not 11/12/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the screen output “Imputing post-discontinuation missing values under MAR:” </t>
+  </si>
+  <si>
+    <t>isn’t quite right as it reports patterns and counts before the interims were imputed - may link to interim problem above?</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -516,25 +532,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -767,27 +764,36 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF0070C0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -811,32 +817,12 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
       </font>
     </dxf>
   </dxfs>
@@ -859,22 +845,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}" name="Table1" displayName="Table1" ref="A2:M26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="2" headerRowBorderDxfId="16" tableBorderDxfId="17">
-  <autoFilter ref="A2:M26" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}" name="Table1" displayName="Table1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
+  <autoFilter ref="A2:M27" xr:uid="{63A6B612-A08F-475A-B68C-2C6A25ECC80C}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F73C437D-1953-40F7-B786-65B34C033CAD}" name="Tester" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{216B41F4-96EB-4AE9-97C9-B7F4F96EA7F8}" name="Mimix version" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{DE5F9776-A5F0-466E-8017-A561894C37CC}" name="Test program" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{740CBD4F-CD6B-43BA-8C70-A1C50399F878}" name="Test" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E66DE38B-E2AE-49D4-96B5-32E818D05F1A}" name="Date" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{BADA15A5-6183-4E6E-9682-948861E68C1C}" name="Passed?" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{1ABFFB10-4F59-4B59-BA12-19132EC5FB73}" name="Finding" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{79B75F80-A7D0-4341-888F-22C9B24CBDB2}" name="Note" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{20595CE3-0CEC-4D84-934E-FB4AC4782736}" name="Action" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{9C26D8EB-E269-4D7C-9FD6-ADC4F8D56709}" name="Status" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{0E207347-9EC9-4313-82AC-B48CBD4EDD88}" name="Date2" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C296EB1B-91E7-458E-AC5C-0C0E20B21231}" name="Passed2" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{5FB8882A-200C-40D3-9158-98279985CFA9}" name="Note2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F73C437D-1953-40F7-B786-65B34C033CAD}" name="Tester" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{216B41F4-96EB-4AE9-97C9-B7F4F96EA7F8}" name="Mimix version" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{DE5F9776-A5F0-466E-8017-A561894C37CC}" name="Test program" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{740CBD4F-CD6B-43BA-8C70-A1C50399F878}" name="Test" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{E66DE38B-E2AE-49D4-96B5-32E818D05F1A}" name="Date" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{BADA15A5-6183-4E6E-9682-948861E68C1C}" name="Passed?" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1ABFFB10-4F59-4B59-BA12-19132EC5FB73}" name="Finding" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{79B75F80-A7D0-4341-888F-22C9B24CBDB2}" name="Note" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{20595CE3-0CEC-4D84-934E-FB4AC4782736}" name="Action" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{9C26D8EB-E269-4D7C-9FD6-ADC4F8D56709}" name="Status" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{0E207347-9EC9-4313-82AC-B48CBD4EDD88}" name="Date2" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{C296EB1B-91E7-458E-AC5C-0C0E20B21231}" name="Passed2" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{5FB8882A-200C-40D3-9158-98279985CFA9}" name="Note2" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1185,13 +1171,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6057EF-99C7-4B7C-82B6-528AB75EDB22}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,13 +2120,44 @@
         <v>100</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="11">
+        <v>44698</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A3:M26">
-    <cfRule type="expression" dxfId="15" priority="1">
+  <conditionalFormatting sqref="A3:M27">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>ISBLANK($L3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$L3="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>